<commit_message>
Update PvZ Heroes Card Database.xlsx
</commit_message>
<xml_diff>
--- a/PvZ Heroes Card Database.xlsx
+++ b/PvZ Heroes Card Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45c9bb75627c78a2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/45c9bb75627c78a2/Desktop/GitHub/PvZHeroes-Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="195" documentId="8_{CD78148F-DF0E-4645-BCBB-F57BBC7739C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1284663E-159E-48B4-8AEB-CF5DA2ABC262}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plants" sheetId="1" r:id="rId1"/>
@@ -4550,11 +4550,11 @@
   </sheetPr>
   <dimension ref="A1:AA977"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -37222,10 +37222,10 @@
   <dimension ref="A1:AB975"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C230" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A253"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -70811,9 +70811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE76972C-F7BB-4769-A2DA-F955752C828E}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -71526,9 +71524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119F6436-4A53-4897-9FD1-3930D7723CA0}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A30"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>